<commit_message>
refactor, add docstrings and type hints
</commit_message>
<xml_diff>
--- a/billing.xlsx
+++ b/billing.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peafly\Documents\Projects\Coding\projects\weekly_projects\monthly_billing_speech_recognition__python\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 

</xml_diff>